<commit_message>
updated btadlp, gbsc, rm with PSP scenario
</commit_message>
<xml_diff>
--- a/InputData/elec/RM/Reserve Margin.xlsx
+++ b/InputData/elec/RM/Reserve Margin.xlsx
@@ -1,26 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI - units progress\InputData\elec\RM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\elec\RM\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F2E58D-FD54-4BA9-89F6-9FCB1A0DDFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="11580"/>
+    <workbookView xWindow="300" yWindow="190" windowWidth="14330" windowHeight="13600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12240" yWindow="110" windowWidth="12840" windowHeight="13600" activeTab="2" xr2:uid="{C6334F97-81B9-476F-A909-EC45C19E39D9}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="RM" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="RM" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>RM Reserve Margin</t>
   </si>
@@ -56,13 +71,100 @@
   </si>
   <si>
     <t>(dimensionless)</t>
+  </si>
+  <si>
+    <t>Planning Reserve Margin Summary</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Peak Load</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>Reserve Margin Requirement</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Total Reserve Margin Requirement (incl. Reliability Adjustments)</t>
+  </si>
+  <si>
+    <t>Firm Capacity</t>
+  </si>
+  <si>
+    <t>CCGT</t>
+  </si>
+  <si>
+    <t>Peaker</t>
+  </si>
+  <si>
+    <t>Steam Turbine</t>
+  </si>
+  <si>
+    <t>CHP</t>
+  </si>
+  <si>
+    <t>Hydro (small + large)</t>
+  </si>
+  <si>
+    <t>Nuclear</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Geothermal</t>
+  </si>
+  <si>
+    <t>Biomass</t>
+  </si>
+  <si>
+    <t>Shed DR</t>
+  </si>
+  <si>
+    <t>Reliability Adjustment (Imports + BTM Resources)</t>
+  </si>
+  <si>
+    <t>Reliability Adjustment (MTR LLT Delay)</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>Battery (incl. BTM)</t>
+  </si>
+  <si>
+    <t>Pumped Storage</t>
+  </si>
+  <si>
+    <t>Variable Renewable ELCC (Incl. BTM)</t>
+  </si>
+  <si>
+    <t>Total Available Capacity</t>
+  </si>
+  <si>
+    <t>Actual Reserve Margin</t>
+  </si>
+  <si>
+    <t>Marginal PRM Cost</t>
+  </si>
+  <si>
+    <t>$/kW-yr.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,13 +180,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -96,19 +211,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -199,6 +318,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -234,6 +370,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -409,21 +562,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -431,42 +585,42 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -478,22 +632,1006 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6C1822-4F94-4F45-9BB9-906ED248FFCD}">
+  <dimension ref="B2:O27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="18.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2023</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2028</v>
+      </c>
+      <c r="K4" s="1">
+        <v>2030</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2032</v>
+      </c>
+      <c r="M4" s="1">
+        <v>2035</v>
+      </c>
+      <c r="N4" s="1">
+        <v>2040</v>
+      </c>
+      <c r="O4" s="1">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>45601.64</v>
+      </c>
+      <c r="F5">
+        <v>45950.43</v>
+      </c>
+      <c r="G5">
+        <v>46607.25</v>
+      </c>
+      <c r="H5">
+        <v>46943.98</v>
+      </c>
+      <c r="I5">
+        <v>47373.33</v>
+      </c>
+      <c r="J5">
+        <v>47801.17</v>
+      </c>
+      <c r="K5">
+        <v>48476.22</v>
+      </c>
+      <c r="L5">
+        <v>49361.88</v>
+      </c>
+      <c r="M5">
+        <v>50955.13</v>
+      </c>
+      <c r="N5">
+        <v>53610.54</v>
+      </c>
+      <c r="O5">
+        <v>56439.35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.225467758820564</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.19950063800975928</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.18324991177455729</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.225467758820564</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0.225467758820564</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0.225467758820564</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0.225467758820564</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0.225467758820564</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0.225467758820564</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>53088.874359999994</v>
+      </c>
+      <c r="F7">
+        <v>53690.264070000005</v>
+      </c>
+      <c r="G7">
+        <v>59069.49220228973</v>
+      </c>
+      <c r="H7">
+        <v>58394.303960717385</v>
+      </c>
+      <c r="I7">
+        <v>58274.488542966988</v>
+      </c>
+      <c r="J7">
+        <v>61011.332668900781</v>
+      </c>
+      <c r="K7">
+        <v>61983.5646794926</v>
+      </c>
+      <c r="L7">
+        <v>63068.912454769619</v>
+      </c>
+      <c r="M7">
+        <v>65021.388961510478</v>
+      </c>
+      <c r="N7">
+        <v>68275.50830296021</v>
+      </c>
+      <c r="O7">
+        <v>71742.123753789405</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>40913.649999999994</v>
+      </c>
+      <c r="F8">
+        <v>41004.590000000004</v>
+      </c>
+      <c r="G8">
+        <v>37263.97</v>
+      </c>
+      <c r="H8">
+        <v>35408.94</v>
+      </c>
+      <c r="I8">
+        <v>35339.929999999993</v>
+      </c>
+      <c r="J8">
+        <v>36221.24</v>
+      </c>
+      <c r="K8">
+        <v>36219.43</v>
+      </c>
+      <c r="L8">
+        <v>35983.93</v>
+      </c>
+      <c r="M8">
+        <v>35617.47</v>
+      </c>
+      <c r="N8">
+        <v>35002.18</v>
+      </c>
+      <c r="O8">
+        <v>35921.280000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>15805.04</v>
+      </c>
+      <c r="F9">
+        <v>15805.04</v>
+      </c>
+      <c r="G9">
+        <v>15805.04</v>
+      </c>
+      <c r="H9">
+        <v>15805.04</v>
+      </c>
+      <c r="I9">
+        <v>15853.43</v>
+      </c>
+      <c r="J9">
+        <v>15853.73</v>
+      </c>
+      <c r="K9">
+        <v>15853.73</v>
+      </c>
+      <c r="L9">
+        <v>15853.73</v>
+      </c>
+      <c r="M9">
+        <v>15853.73</v>
+      </c>
+      <c r="N9">
+        <v>15853.73</v>
+      </c>
+      <c r="O9">
+        <v>16733.080000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <v>8161.21</v>
+      </c>
+      <c r="F10">
+        <v>8161.21</v>
+      </c>
+      <c r="G10">
+        <v>8161.21</v>
+      </c>
+      <c r="H10">
+        <v>7887.2699999999995</v>
+      </c>
+      <c r="I10">
+        <v>7793.87</v>
+      </c>
+      <c r="J10">
+        <v>7793.93</v>
+      </c>
+      <c r="K10">
+        <v>7793.94</v>
+      </c>
+      <c r="L10">
+        <v>7793.94</v>
+      </c>
+      <c r="M10">
+        <v>7793.94</v>
+      </c>
+      <c r="N10">
+        <v>7793.94</v>
+      </c>
+      <c r="O10">
+        <v>7793.93</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <v>2860.59</v>
+      </c>
+      <c r="F11">
+        <v>2860.59</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <v>1365.87</v>
+      </c>
+      <c r="F12">
+        <v>1341.45</v>
+      </c>
+      <c r="G12">
+        <v>1311.45</v>
+      </c>
+      <c r="H12">
+        <v>1243.03</v>
+      </c>
+      <c r="I12">
+        <v>1177.5</v>
+      </c>
+      <c r="J12">
+        <v>1177.5</v>
+      </c>
+      <c r="K12">
+        <v>1177.5</v>
+      </c>
+      <c r="L12">
+        <v>942</v>
+      </c>
+      <c r="M12">
+        <v>588.75</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13">
+        <v>5205.5300000000007</v>
+      </c>
+      <c r="F13">
+        <v>5205.5300000000007</v>
+      </c>
+      <c r="G13">
+        <v>5205.5300000000007</v>
+      </c>
+      <c r="H13">
+        <v>5205.5300000000007</v>
+      </c>
+      <c r="I13">
+        <v>5205.5300000000007</v>
+      </c>
+      <c r="J13">
+        <v>5205.5300000000007</v>
+      </c>
+      <c r="K13">
+        <v>5205.13</v>
+      </c>
+      <c r="L13">
+        <v>5205.13</v>
+      </c>
+      <c r="M13">
+        <v>5205.13</v>
+      </c>
+      <c r="N13">
+        <v>5205.13</v>
+      </c>
+      <c r="O13">
+        <v>5205.13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14">
+        <v>2915</v>
+      </c>
+      <c r="F14">
+        <v>2915</v>
+      </c>
+      <c r="G14">
+        <v>1772.84</v>
+      </c>
+      <c r="H14">
+        <v>630.66999999999996</v>
+      </c>
+      <c r="I14">
+        <v>630.66999999999996</v>
+      </c>
+      <c r="J14">
+        <v>630.66999999999996</v>
+      </c>
+      <c r="K14">
+        <v>630.66999999999996</v>
+      </c>
+      <c r="L14">
+        <v>630.66999999999996</v>
+      </c>
+      <c r="M14">
+        <v>630.66999999999996</v>
+      </c>
+      <c r="N14">
+        <v>630.66999999999996</v>
+      </c>
+      <c r="O14">
+        <v>630.66999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15">
+        <v>479</v>
+      </c>
+      <c r="F15">
+        <v>479</v>
+      </c>
+      <c r="G15">
+        <v>479</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>1214.5199999999998</v>
+      </c>
+      <c r="F16">
+        <v>1302.6199999999999</v>
+      </c>
+      <c r="G16">
+        <v>1302.6199999999999</v>
+      </c>
+      <c r="H16">
+        <v>1302.6199999999999</v>
+      </c>
+      <c r="I16">
+        <v>1365.5999999999997</v>
+      </c>
+      <c r="J16">
+        <v>2202.1999999999998</v>
+      </c>
+      <c r="K16">
+        <v>2202.1999999999998</v>
+      </c>
+      <c r="L16">
+        <v>2202.1999999999998</v>
+      </c>
+      <c r="M16">
+        <v>2202.1999999999998</v>
+      </c>
+      <c r="N16">
+        <v>2202.1999999999998</v>
+      </c>
+      <c r="O16">
+        <v>2202.1999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>636.39</v>
+      </c>
+      <c r="F17">
+        <v>662.86</v>
+      </c>
+      <c r="G17">
+        <v>678.27</v>
+      </c>
+      <c r="H17">
+        <v>698.67000000000007</v>
+      </c>
+      <c r="I17">
+        <v>698.67000000000007</v>
+      </c>
+      <c r="J17">
+        <v>721.57</v>
+      </c>
+      <c r="K17">
+        <v>720.15</v>
+      </c>
+      <c r="L17">
+        <v>720.15</v>
+      </c>
+      <c r="M17">
+        <v>720.15</v>
+      </c>
+      <c r="N17">
+        <v>720.15</v>
+      </c>
+      <c r="O17">
+        <v>720.16</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18">
+        <v>2270.5</v>
+      </c>
+      <c r="F18">
+        <v>2271.29</v>
+      </c>
+      <c r="G18">
+        <v>2548.0099999999998</v>
+      </c>
+      <c r="H18">
+        <v>2636.1099999999997</v>
+      </c>
+      <c r="I18">
+        <v>2614.66</v>
+      </c>
+      <c r="J18">
+        <v>2636.1099999999997</v>
+      </c>
+      <c r="K18">
+        <v>2636.1099999999997</v>
+      </c>
+      <c r="L18">
+        <v>2636.1099999999997</v>
+      </c>
+      <c r="M18">
+        <v>2622.8999999999996</v>
+      </c>
+      <c r="N18">
+        <v>2596.3599999999997</v>
+      </c>
+      <c r="O18">
+        <v>2636.1099999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19">
+        <v>-692.59</v>
+      </c>
+      <c r="F19">
+        <v>-893.22</v>
+      </c>
+      <c r="G19">
+        <v>-1953.81</v>
+      </c>
+      <c r="H19">
+        <v>-2084.9700000000003</v>
+      </c>
+      <c r="I19">
+        <v>-2220</v>
+      </c>
+      <c r="J19">
+        <v>-2432.54</v>
+      </c>
+      <c r="K19">
+        <v>-2577.52</v>
+      </c>
+      <c r="L19">
+        <v>-2577.52</v>
+      </c>
+      <c r="M19">
+        <v>-2577.52</v>
+      </c>
+      <c r="N19">
+        <v>-2577.52</v>
+      </c>
+      <c r="O19">
+        <v>-2577.52</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20">
+        <v>-1219</v>
+      </c>
+      <c r="I20">
+        <v>-2000</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21">
+        <v>4806.71</v>
+      </c>
+      <c r="F21">
+        <v>6142.08</v>
+      </c>
+      <c r="G21">
+        <v>12745.08</v>
+      </c>
+      <c r="H21">
+        <v>13864.29</v>
+      </c>
+      <c r="I21">
+        <v>13772.62</v>
+      </c>
+      <c r="J21">
+        <v>15420.93</v>
+      </c>
+      <c r="K21">
+        <v>15671.720000000001</v>
+      </c>
+      <c r="L21">
+        <v>16442.849999999999</v>
+      </c>
+      <c r="M21">
+        <v>18674.84</v>
+      </c>
+      <c r="N21">
+        <v>22437.74</v>
+      </c>
+      <c r="O21">
+        <v>24380.48</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22">
+        <v>2908.21</v>
+      </c>
+      <c r="F22">
+        <v>4243.58</v>
+      </c>
+      <c r="G22">
+        <v>10846.58</v>
+      </c>
+      <c r="H22">
+        <v>11965.79</v>
+      </c>
+      <c r="I22">
+        <v>11694.45</v>
+      </c>
+      <c r="J22">
+        <v>12522.43</v>
+      </c>
+      <c r="K22">
+        <v>12772.94</v>
+      </c>
+      <c r="L22">
+        <v>13544.07</v>
+      </c>
+      <c r="M22">
+        <v>15799.94</v>
+      </c>
+      <c r="N22">
+        <v>19621.240000000002</v>
+      </c>
+      <c r="O22">
+        <v>21481.7</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23">
+        <v>1898.5</v>
+      </c>
+      <c r="F23">
+        <v>1898.5</v>
+      </c>
+      <c r="G23">
+        <v>1898.5</v>
+      </c>
+      <c r="H23">
+        <v>1898.5</v>
+      </c>
+      <c r="I23">
+        <v>2078.17</v>
+      </c>
+      <c r="J23">
+        <v>2898.5</v>
+      </c>
+      <c r="K23">
+        <v>2898.7799999999997</v>
+      </c>
+      <c r="L23">
+        <v>2898.7799999999997</v>
+      </c>
+      <c r="M23">
+        <v>2874.8999999999996</v>
+      </c>
+      <c r="N23">
+        <v>2816.5</v>
+      </c>
+      <c r="O23">
+        <v>2898.7799999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24">
+        <v>8898.77</v>
+      </c>
+      <c r="F24">
+        <v>8968.26</v>
+      </c>
+      <c r="G24">
+        <v>9060.4699999999993</v>
+      </c>
+      <c r="H24">
+        <v>9121.08</v>
+      </c>
+      <c r="I24">
+        <v>9254.66</v>
+      </c>
+      <c r="J24">
+        <v>9369.15</v>
+      </c>
+      <c r="K24">
+        <v>10092.42</v>
+      </c>
+      <c r="L24">
+        <v>10642.14</v>
+      </c>
+      <c r="M24">
+        <v>10788</v>
+      </c>
+      <c r="N24">
+        <v>11159.54</v>
+      </c>
+      <c r="O24">
+        <v>11440.37</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25">
+        <v>53926.539999999994</v>
+      </c>
+      <c r="F25">
+        <v>55221.710000000006</v>
+      </c>
+      <c r="G25">
+        <v>57115.710000000006</v>
+      </c>
+      <c r="H25">
+        <v>56309.340000000004</v>
+      </c>
+      <c r="I25">
+        <v>56147.209999999992</v>
+      </c>
+      <c r="J25">
+        <v>58578.78</v>
+      </c>
+      <c r="K25">
+        <v>59406.05</v>
+      </c>
+      <c r="L25">
+        <v>60491.4</v>
+      </c>
+      <c r="M25">
+        <v>62502.790000000008</v>
+      </c>
+      <c r="N25">
+        <v>66021.94</v>
+      </c>
+      <c r="O25">
+        <v>69164.61</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26">
+        <v>0.18255703084362751</v>
+      </c>
+      <c r="F26">
+        <v>0.20176699108147633</v>
+      </c>
+      <c r="G26">
+        <v>0.2254683552451604</v>
+      </c>
+      <c r="H26">
+        <v>0.19950076665847249</v>
+      </c>
+      <c r="I26">
+        <v>0.18520716192000841</v>
+      </c>
+      <c r="J26">
+        <v>0.22546749378728603</v>
+      </c>
+      <c r="K26">
+        <v>0.22546786857556134</v>
+      </c>
+      <c r="L26">
+        <v>0.22546791167597346</v>
+      </c>
+      <c r="M26">
+        <v>0.22662409064602551</v>
+      </c>
+      <c r="N26">
+        <v>0.23151044552060096</v>
+      </c>
+      <c r="O26">
+        <v>0.22546786949176423</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F27">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G27">
+        <v>273.32565999999997</v>
+      </c>
+      <c r="H27">
+        <v>527.63913000000002</v>
+      </c>
+      <c r="I27">
+        <v>7.0000000000000007E-5</v>
+      </c>
+      <c r="J27">
+        <v>216.50995999999998</v>
+      </c>
+      <c r="K27">
+        <v>71.152160000000009</v>
+      </c>
+      <c r="L27">
+        <v>21.935400000000001</v>
+      </c>
+      <c r="M27">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="N27">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="O27">
+        <v>74.562080000000009</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AK2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -606,117 +1744,153 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" ref="B2:G2" si="0">C2</f>
+        <v>0.14899999999999999</v>
       </c>
       <c r="C2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.14899999999999999</v>
       </c>
       <c r="D2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.14899999999999999</v>
       </c>
       <c r="E2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.14899999999999999</v>
       </c>
       <c r="F2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.14899999999999999</v>
       </c>
       <c r="G2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.14899999999999999</v>
       </c>
       <c r="H2" s="3">
-        <v>0.14119999999999999</v>
+        <f>I2</f>
+        <v>0.14899999999999999</v>
       </c>
       <c r="I2" s="3">
-        <v>0.14119999999999999</v>
+        <f>Sheet1!E6</f>
+        <v>0.14899999999999999</v>
       </c>
       <c r="J2" s="3">
-        <v>0.14119999999999999</v>
+        <f>Sheet1!F6</f>
+        <v>0.14899999999999999</v>
       </c>
       <c r="K2" s="3">
-        <v>0.14119999999999999</v>
+        <f>Sheet1!G6</f>
+        <v>0.225467758820564</v>
       </c>
       <c r="L2" s="3">
-        <v>0.14119999999999999</v>
+        <f>Sheet1!H6</f>
+        <v>0.19950063800975928</v>
       </c>
       <c r="M2" s="3">
-        <v>0.14119999999999999</v>
+        <f>Sheet1!I6</f>
+        <v>0.18324991177455729</v>
       </c>
       <c r="N2" s="3">
-        <v>0.14119999999999999</v>
+        <f>Sheet1!J6</f>
+        <v>0.225467758820564</v>
       </c>
       <c r="O2" s="3">
-        <v>0.14119999999999999</v>
+        <f>N2</f>
+        <v>0.225467758820564</v>
       </c>
       <c r="P2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" ref="P2:AK2" si="1">O2</f>
+        <v>0.225467758820564</v>
       </c>
       <c r="Q2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="R2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="S2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="T2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="U2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="V2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="W2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="X2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="Y2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="Z2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="AA2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="AB2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="AC2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="AD2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="AE2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="AF2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="AG2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="AH2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="AI2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="AJ2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
       <c r="AK2" s="3">
-        <v>0.14119999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.225467758820564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>